<commit_message>
Add changes in test
</commit_message>
<xml_diff>
--- a/Тестировка.xlsx
+++ b/Тестировка.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87526F85-A861-4B71-8E01-54C69441053F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D15201D4-8447-4AFB-B2F3-EB706404FD1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
   <si>
     <t>Номер</t>
   </si>
@@ -131,6 +131,12 @@
   </si>
   <si>
     <t>Специальность добавлена в бд и отображена в таблице.Специальность, имеющий связь с другими объектами бд, не удаляется, если связи нет - удаление успешно. Редактирование происходит успешно для всех объектов</t>
+  </si>
+  <si>
+    <t>Итак, проведя ряд тестов , можно сделать вывод, что проект не готов. Функциональные требования учтены все, но не выполняют должного.</t>
+  </si>
+  <si>
+    <t>Выполнил Гаврилов А.Д. для проекта Дубровина</t>
   </si>
 </sst>
 </file>
@@ -154,7 +160,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -162,21 +168,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -454,180 +478,208 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="75.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="43.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="71.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="43.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="26.7109375" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="6.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="75.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="43.5546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="71.44140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="43.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="26.6640625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F4" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F5" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+    <row r="6" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F6" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+    <row r="7" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F7" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+    <row r="8" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C8" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F8" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1" t="s">
+    <row r="9" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E9" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F9" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1" t="s">
+    <row r="10" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D10" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E10" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F10" s="3" t="s">
         <v>22</v>
       </c>
     </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B11" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A12:B14"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>